<commit_message>
Repgrid funcional, procesado del xlsx
</commit_message>
<xml_diff>
--- a/ficheros/excel_rep.xlsx
+++ b/ficheros/excel_rep.xlsx
@@ -44,13 +44,13 @@
     <t xml:space="preserve">Gabi</t>
   </si>
   <si>
-    <t xml:space="preserve">Angela</t>
+    <t xml:space="preserve">Ángela</t>
   </si>
   <si>
     <t xml:space="preserve">Mara</t>
   </si>
   <si>
-    <t xml:space="preserve">Rocio</t>
+    <t xml:space="preserve">Acéntón</t>
   </si>
   <si>
     <t xml:space="preserve">Yo - Ideal </t>
@@ -62,18 +62,18 @@
     <t xml:space="preserve">Tranquilo</t>
   </si>
   <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ansioso</t>
   </si>
   <si>
@@ -143,13 +143,13 @@
     <t xml:space="preserve">Apagado</t>
   </si>
   <si>
-    <t xml:space="preserve">Energico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egocentrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empatico</t>
+    <t xml:space="preserve">Enérgico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egocéntrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empático</t>
   </si>
   <si>
     <t xml:space="preserve">Asocial</t>
@@ -164,10 +164,10 @@
     <t xml:space="preserve">Concienciado</t>
   </si>
   <si>
-    <t xml:space="preserve">Frio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calido</t>
+    <t xml:space="preserve">Frío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cálido</t>
   </si>
   <si>
     <t xml:space="preserve">No curioso</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Curioso</t>
   </si>
   <si>
-    <t xml:space="preserve">Antipatico</t>
+    <t xml:space="preserve">Antipático</t>
   </si>
   <si>
     <t xml:space="preserve">Amable</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">Agradable</t>
   </si>
   <si>
-    <t xml:space="preserve">Grunyon</t>
+    <t xml:space="preserve">Gruñón</t>
   </si>
   <si>
     <t xml:space="preserve">Complaciente</t>
@@ -587,40 +587,40 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
         <v>0</v>
@@ -634,22 +634,22 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -658,16 +658,16 @@
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -681,40 +681,40 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N4" t="s">
         <v>24</v>
@@ -728,25 +728,25 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -758,13 +758,13 @@
         <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O5" t="s">
         <v>27</v>
@@ -775,10 +775,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -790,28 +790,28 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
         <v>29</v>
@@ -822,43 +822,43 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>
@@ -869,13 +869,13 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -884,28 +884,28 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O8" t="s">
         <v>33</v>
@@ -916,40 +916,40 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -963,40 +963,40 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
@@ -1013,7 +1013,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1022,31 +1022,31 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" t="s">
         <v>39</v>
@@ -1057,7 +1057,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1069,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -1081,19 +1081,19 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K12" t="s">
         <v>24</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O12" t="s">
         <v>41</v>
@@ -1107,10 +1107,10 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1119,28 +1119,28 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
         <v>14</v>
       </c>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O13" t="s">
         <v>43</v>
@@ -1151,40 +1151,40 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
@@ -1198,10 +1198,10 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -1213,28 +1213,28 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O15" t="s">
         <v>47</v>
@@ -1245,10 +1245,10 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -1257,28 +1257,28 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
@@ -1292,40 +1292,40 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
@@ -1339,13 +1339,13 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -1354,22 +1354,22 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" t="s">
         <v>14</v>
       </c>
       <c r="L18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -1386,25 +1386,25 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
         <v>14</v>
@@ -1416,10 +1416,10 @@
         <v>14</v>
       </c>
       <c r="L19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N19" t="s">
         <v>14</v>
@@ -1433,16 +1433,16 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
@@ -1463,13 +1463,13 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O20" t="s">
         <v>57</v>
@@ -1480,7 +1480,7 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -1489,16 +1489,16 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" t="s">
         <v>24</v>
@@ -1507,16 +1507,16 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O21" t="s">
         <v>59</v>
@@ -1539,31 +1539,31 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
       </c>
       <c r="N22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O22" t="s">
         <v>61</v>
@@ -1583,31 +1583,31 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N23" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Mejora actualización tablas pacientes y fechas simulaciones. Títulos reactivos de las simulaciones y empezando wimpgrid
</commit_message>
<xml_diff>
--- a/ficheros/excel_rep.xlsx
+++ b/ficheros/excel_rep.xlsx
@@ -44,13 +44,13 @@
     <t xml:space="preserve">Gabi</t>
   </si>
   <si>
-    <t xml:space="preserve">Ángela</t>
+    <t xml:space="preserve">Angela</t>
   </si>
   <si>
     <t xml:space="preserve">Mara</t>
   </si>
   <si>
-    <t xml:space="preserve">Acéntón</t>
+    <t xml:space="preserve">Rocio</t>
   </si>
   <si>
     <t xml:space="preserve">Yo - Ideal </t>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">Tranquilo</t>
   </si>
   <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
@@ -71,9 +74,6 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ansioso</t>
   </si>
   <si>
@@ -143,13 +143,13 @@
     <t xml:space="preserve">Apagado</t>
   </si>
   <si>
-    <t xml:space="preserve">Enérgico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egocéntrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empático</t>
+    <t xml:space="preserve">Energico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egocentrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empatico</t>
   </si>
   <si>
     <t xml:space="preserve">Asocial</t>
@@ -164,10 +164,10 @@
     <t xml:space="preserve">Concienciado</t>
   </si>
   <si>
-    <t xml:space="preserve">Frío</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cálido</t>
+    <t xml:space="preserve">Frio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calido</t>
   </si>
   <si>
     <t xml:space="preserve">No curioso</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Curioso</t>
   </si>
   <si>
-    <t xml:space="preserve">Antipático</t>
+    <t xml:space="preserve">Antipatico</t>
   </si>
   <si>
     <t xml:space="preserve">Amable</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">Agradable</t>
   </si>
   <si>
-    <t xml:space="preserve">Gruñón</t>
+    <t xml:space="preserve">Grunyon</t>
   </si>
   <si>
     <t xml:space="preserve">Complaciente</t>
@@ -587,40 +587,40 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
         <v>0</v>
@@ -634,22 +634,22 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -658,16 +658,16 @@
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -681,40 +681,40 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" t="s">
         <v>24</v>
@@ -728,25 +728,25 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -758,13 +758,13 @@
         <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O5" t="s">
         <v>27</v>
@@ -775,10 +775,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -790,28 +790,28 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O6" t="s">
         <v>29</v>
@@ -822,43 +822,43 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>
@@ -869,13 +869,13 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -884,28 +884,28 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>33</v>
@@ -916,40 +916,40 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -963,40 +963,40 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10" t="s">
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
@@ -1013,7 +1013,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1022,31 +1022,31 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
       </c>
       <c r="M11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O11" t="s">
         <v>39</v>
@@ -1057,7 +1057,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1069,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -1081,19 +1081,19 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
         <v>24</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O12" t="s">
         <v>41</v>
@@ -1107,10 +1107,10 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1119,28 +1119,28 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s">
         <v>14</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O13" t="s">
         <v>43</v>
@@ -1151,40 +1151,40 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
@@ -1198,10 +1198,10 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -1213,28 +1213,28 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O15" t="s">
         <v>47</v>
@@ -1245,10 +1245,10 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -1257,28 +1257,28 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
@@ -1292,40 +1292,40 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
@@ -1339,13 +1339,13 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -1354,22 +1354,22 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K18" t="s">
         <v>14</v>
       </c>
       <c r="L18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -1386,25 +1386,25 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s">
         <v>14</v>
@@ -1416,10 +1416,10 @@
         <v>14</v>
       </c>
       <c r="L19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N19" t="s">
         <v>14</v>
@@ -1433,16 +1433,16 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
@@ -1463,13 +1463,13 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O20" t="s">
         <v>57</v>
@@ -1480,7 +1480,7 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -1489,16 +1489,16 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
         <v>24</v>
@@ -1507,16 +1507,16 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O21" t="s">
         <v>59</v>
@@ -1539,31 +1539,31 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
       </c>
       <c r="N22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O22" t="s">
         <v>61</v>
@@ -1583,31 +1583,31 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N23" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Arreglado bugs render tables. Warning al borrar paciente
</commit_message>
<xml_diff>
--- a/ficheros/excel_rep.xlsx
+++ b/ficheros/excel_rep.xlsx
@@ -12,45 +12,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">Yo - Actual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Padre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hermano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jairo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rocio</t>
+    <t xml:space="preserve">Yo - Totalmente Ansioso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente No deportista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Vive el presente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Trabajador </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Rodeado de gente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Libre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Ordenado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Idiota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Triste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente proactivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Flexible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Enérgico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Egocéntrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Sociable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente No concienciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Frío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente No curioso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Antipático</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Alegre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Asertivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Busca Apoyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yo - Totalmente Enfrentado los problemas</t>
   </si>
   <si>
     <t xml:space="preserve">Yo - Ideal </t>
@@ -65,30 +95,30 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
+    <t xml:space="preserve">Ansioso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No deportista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deportista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vive presente</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">Ansioso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No deportista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deportista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vive presente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proyecta a futuro</t>
   </si>
   <si>
@@ -143,13 +173,13 @@
     <t xml:space="preserve">Apagado</t>
   </si>
   <si>
-    <t xml:space="preserve">Energico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egocentrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empatico</t>
+    <t xml:space="preserve">Enérgico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egocéntrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empático</t>
   </si>
   <si>
     <t xml:space="preserve">Asocial</t>
@@ -164,10 +194,10 @@
     <t xml:space="preserve">Concienciado</t>
   </si>
   <si>
-    <t xml:space="preserve">Frio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calido</t>
+    <t xml:space="preserve">Frío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cálido</t>
   </si>
   <si>
     <t xml:space="preserve">No curioso</t>
@@ -176,7 +206,7 @@
     <t xml:space="preserve">Curioso</t>
   </si>
   <si>
-    <t xml:space="preserve">Antipatico</t>
+    <t xml:space="preserve">Antipático</t>
   </si>
   <si>
     <t xml:space="preserve">Amable</t>
@@ -185,7 +215,7 @@
     <t xml:space="preserve">Agradable</t>
   </si>
   <si>
-    <t xml:space="preserve">Grunyon</t>
+    <t xml:space="preserve">Gruñón</t>
   </si>
   <si>
     <t xml:space="preserve">Complaciente</t>
@@ -581,1039 +611,1729 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U6" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="N8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="N9" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="O9" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" t="s">
+        <v>29</v>
+      </c>
+      <c r="V9" t="s">
+        <v>29</v>
+      </c>
+      <c r="W9" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N10" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="O10" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="P10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" t="s">
+        <v>28</v>
+      </c>
+      <c r="X10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="O11" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="O12" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="P12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="M13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N13" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="O13" t="s">
-        <v>43</v>
+        <v>28</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" t="s">
+        <v>27</v>
+      </c>
+      <c r="V13" t="s">
+        <v>27</v>
+      </c>
+      <c r="W13" t="s">
+        <v>27</v>
+      </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L14" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="M14" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="O14" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="P14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" t="s">
+        <v>29</v>
+      </c>
+      <c r="V14" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" t="s">
+        <v>29</v>
+      </c>
+      <c r="X14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="M15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="N15" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="O15" t="s">
-        <v>47</v>
+        <v>34</v>
+      </c>
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" t="s">
+        <v>34</v>
+      </c>
+      <c r="S15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T15" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15" t="s">
+        <v>34</v>
+      </c>
+      <c r="V15" t="s">
+        <v>34</v>
+      </c>
+      <c r="W15" t="s">
+        <v>34</v>
+      </c>
+      <c r="X15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="L16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="M16" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="N16" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="P16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U16" t="s">
+        <v>28</v>
+      </c>
+      <c r="V16" t="s">
+        <v>28</v>
+      </c>
+      <c r="W16" t="s">
+        <v>24</v>
+      </c>
+      <c r="X16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="L17" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M17" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="N17" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="O17" t="s">
-        <v>51</v>
+        <v>24</v>
+      </c>
+      <c r="P17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" t="s">
+        <v>29</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>24</v>
+      </c>
+      <c r="U17" t="s">
+        <v>28</v>
+      </c>
+      <c r="V17" t="s">
+        <v>29</v>
+      </c>
+      <c r="W17" t="s">
+        <v>29</v>
+      </c>
+      <c r="X17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="K18" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="M18" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="N18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="O18" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="P18" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18" t="s">
+        <v>29</v>
+      </c>
+      <c r="V18" t="s">
+        <v>29</v>
+      </c>
+      <c r="W18" t="s">
+        <v>29</v>
+      </c>
+      <c r="X18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="J19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="K19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="L19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="M19" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N19" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>55</v>
+        <v>24</v>
+      </c>
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" t="s">
+        <v>24</v>
+      </c>
+      <c r="U19" t="s">
+        <v>29</v>
+      </c>
+      <c r="V19" t="s">
+        <v>29</v>
+      </c>
+      <c r="W19" t="s">
+        <v>29</v>
+      </c>
+      <c r="X19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="I20" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="L20" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="N20" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="O20" t="s">
-        <v>57</v>
+        <v>26</v>
+      </c>
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20" t="s">
+        <v>29</v>
+      </c>
+      <c r="T20" t="s">
+        <v>34</v>
+      </c>
+      <c r="U20" t="s">
+        <v>28</v>
+      </c>
+      <c r="V20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20" t="s">
+        <v>34</v>
+      </c>
+      <c r="X20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J21" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="L21" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="N21" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O21" t="s">
-        <v>59</v>
+        <v>26</v>
+      </c>
+      <c r="P21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" t="s">
+        <v>34</v>
+      </c>
+      <c r="S21" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U21" t="s">
+        <v>34</v>
+      </c>
+      <c r="V21" t="s">
+        <v>34</v>
+      </c>
+      <c r="W21" t="s">
+        <v>29</v>
+      </c>
+      <c r="X21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M22" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="N22" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" t="s">
+        <v>27</v>
+      </c>
+      <c r="T22" t="s">
+        <v>27</v>
+      </c>
+      <c r="U22" t="s">
+        <v>27</v>
+      </c>
+      <c r="V22" t="s">
+        <v>27</v>
+      </c>
+      <c r="W22" t="s">
+        <v>28</v>
+      </c>
+      <c r="X22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I23" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="L23" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M23" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="N23" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="O23" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>27</v>
+      </c>
+      <c r="R23" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" t="s">
+        <v>27</v>
+      </c>
+      <c r="U23" t="s">
+        <v>28</v>
+      </c>
+      <c r="V23" t="s">
+        <v>29</v>
+      </c>
+      <c r="W23" t="s">
+        <v>27</v>
+      </c>
+      <c r="X23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado bugs importar siempre la misma rejilla
</commit_message>
<xml_diff>
--- a/ficheros/excel_rep.xlsx
+++ b/ficheros/excel_rep.xlsx
@@ -44,13 +44,13 @@
     <t xml:space="preserve">Gabi</t>
   </si>
   <si>
-    <t xml:space="preserve">Ángela</t>
+    <t xml:space="preserve">Angela</t>
   </si>
   <si>
     <t xml:space="preserve">Mara</t>
   </si>
   <si>
-    <t xml:space="preserve">Rocío</t>
+    <t xml:space="preserve">Rocio</t>
   </si>
   <si>
     <t xml:space="preserve">Yo - Ideal </t>
@@ -143,13 +143,13 @@
     <t xml:space="preserve">Apagado</t>
   </si>
   <si>
-    <t xml:space="preserve">Enérgico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egocéntrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empático</t>
+    <t xml:space="preserve">Energico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egocentrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empatico</t>
   </si>
   <si>
     <t xml:space="preserve">Asocial</t>
@@ -164,10 +164,10 @@
     <t xml:space="preserve">Concienciado</t>
   </si>
   <si>
-    <t xml:space="preserve">Frío</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cálido</t>
+    <t xml:space="preserve">Frio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calido</t>
   </si>
   <si>
     <t xml:space="preserve">No curioso</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Curioso</t>
   </si>
   <si>
-    <t xml:space="preserve">Antipático</t>
+    <t xml:space="preserve">Antipatico</t>
   </si>
   <si>
     <t xml:space="preserve">Amable</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">Agradable</t>
   </si>
   <si>
-    <t xml:space="preserve">Gruñón</t>
+    <t xml:space="preserve">Grunyon</t>
   </si>
   <si>
     <t xml:space="preserve">Complaciente</t>

</xml_diff>